<commit_message>
Order by changes in masters, edit mode updation in post operation and pakaging master and some name changes in masters
</commit_message>
<xml_diff>
--- a/PB ERP - FEEDBACK.xlsx
+++ b/PB ERP - FEEDBACK.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ERP_Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029597AE-0091-45FE-8B23-3F2D5214253B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B11F0A-E77E-47E3-9A13-377F254EE7CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6915C726-160E-4E45-A63C-2B463591B386}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{6915C726-160E-4E45-A63C-2B463591B386}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="49">
   <si>
     <t>ASSEMBLY OPN RECORDING WITH CHILD PARTS</t>
   </si>
@@ -125,9 +125,6 @@
     <t>DPR REPORT</t>
   </si>
   <si>
-    <t>REMARKS</t>
-  </si>
-  <si>
     <t>OPEN</t>
   </si>
   <si>
@@ -162,6 +159,30 @@
   </si>
   <si>
     <t>DPR LIST DATE WISE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>DEVELOPER'S REMARK</t>
+  </si>
+  <si>
+    <t>REMARK</t>
+  </si>
+  <si>
+    <t>PROCESS</t>
+  </si>
+  <si>
+    <t>ORDER BY MASTERS</t>
+  </si>
+  <si>
+    <t>UPDATING IN POST/PACKAGING REQUIRED WHEN PART EDITED</t>
+  </si>
+  <si>
+    <t>FPA LIST DELETE OPTION</t>
+  </si>
+  <si>
+    <t>FPA</t>
   </si>
 </sst>
 </file>
@@ -232,11 +253,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,35 +573,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A5FD1A-4852-47E6-9682-43E522F06F28}">
-  <dimension ref="A1:E31"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.85546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="21.7109375" style="1"/>
+    <col min="1" max="1" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.21875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="21.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="1">
         <f>SUBTOTAL(3,E3:E277)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -591,10 +613,13 @@
         <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -608,10 +633,10 @@
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -625,10 +650,10 @@
         <v>22</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -636,16 +661,19 @@
         <v>43854</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -659,10 +687,10 @@
         <v>22</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -676,10 +704,13 @@
         <v>22</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -693,10 +724,10 @@
         <v>22</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -710,27 +741,30 @@
         <v>22</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
       <c r="B10" s="4">
         <v>43854</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -744,10 +778,10 @@
         <v>22</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -761,10 +795,10 @@
         <v>22</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -778,10 +812,13 @@
         <v>23</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>12</v>
       </c>
@@ -792,13 +829,16 @@
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -812,10 +852,10 @@
         <v>23</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>14</v>
       </c>
@@ -823,16 +863,19 @@
         <v>43854</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -843,13 +886,16 @@
         <v>6</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>16</v>
       </c>
@@ -863,10 +909,13 @@
         <v>23</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>17</v>
       </c>
@@ -880,10 +929,13 @@
         <v>23</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>18</v>
       </c>
@@ -897,10 +949,10 @@
         <v>23</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>19</v>
       </c>
@@ -908,50 +960,59 @@
         <v>43854</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>43854</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>43854</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>33</v>
+      <c r="C23" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>22</v>
       </c>
@@ -959,13 +1020,16 @@
         <v>43854</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>23</v>
       </c>
@@ -979,10 +1043,13 @@
         <v>26</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>24</v>
       </c>
@@ -990,16 +1057,16 @@
         <v>43882</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>25</v>
       </c>
@@ -1007,16 +1074,16 @@
         <v>43883</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>26</v>
       </c>
@@ -1024,32 +1091,98 @@
         <v>43883</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+        <v>29</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="2"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="2"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="2"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+      <c r="B32" s="4">
+        <v>43887</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+      <c r="B33" s="4">
+        <v>43887</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>29</v>
+      </c>
+      <c r="B34" s="4">
+        <v>43887</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E31" xr:uid="{6E1326A4-CAE6-4106-BA1A-0CB4756777A0}"/>
+  <autoFilter ref="A2:E31" xr:uid="{6E1326A4-CAE6-4106-BA1A-0CB4756777A0}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="OPEN"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>

</xml_diff>